<commit_message>
v1.2 Update für Mupibox v4.0.4
Attribute für Mupibox Version 4.0.4 angepasst, Template Excel Datei aktualisiert, Spaltenbezeichnung vereinheitlicht, fixed https://github.com/Feuer-sturm/MuPiBox_MusikVerwaltung/issues/3
</commit_message>
<xml_diff>
--- a/sample_data/MuPiBox_MusikVerwaltung_Template.xlsx
+++ b/sample_data/MuPiBox_MusikVerwaltung_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Github_Repository\MuPiBox_MusikVerwaltung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Github_Repository\MuPiBox_MusikVerwaltung\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911774CF-3702-4DEE-8278-B7D78E431AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFFAC92-7D72-431C-943B-D1EC373DAA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="MuPibox" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MuPibox!$A$2:$R$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MuPibox!$A$2:$R$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="135">
   <si>
     <t>https://open.spotify.com/album/7EPQEUgL5LbEDIRqc5YARW?si=sJFY_H0RSSuSyeObYRHDFg</t>
   </si>
@@ -90,18 +90,6 @@
     <t>Connie</t>
   </si>
   <si>
-    <t>5UkoCFXGVib8TIc8cvKtfq?si=NblVGGPGRISgLeOVeZtDsQ</t>
-  </si>
-  <si>
-    <t>3626UDwiaF1YhpqqSn1Deh?si=HWjuIfO2QL2HNqOxinVUPg</t>
-  </si>
-  <si>
-    <t>6bZnwwe52KE9uDlVNQhnyz?si=ymBs7sQNRIqQ3tTaWl3vkg</t>
-  </si>
-  <si>
-    <t>6ldqnwRlLHxc5qAUCfLm2P?si=hdlmNeNRRn-kWlS3Nh98Hw</t>
-  </si>
-  <si>
     <t>Paw Patrol</t>
   </si>
   <si>
@@ -111,9 +99,6 @@
     <t>Regenbogen Fisch</t>
   </si>
   <si>
-    <t>029DikZUQus7AGcU2n71tb?si=IJaMqOufRiO8Quro8oyXPQ</t>
-  </si>
-  <si>
     <t>add to file</t>
   </si>
   <si>
@@ -132,63 +117,24 @@
     <t>https://open.spotify.com/album/029DikZUQus7AGcU2n71tb?si=IJaMqOufRiO8Quro8oyXPQ</t>
   </si>
   <si>
-    <t>7EPQEUgL5LbEDIRqc5YARW?si=sJFY_H0RSSuSyeObYRHDFg</t>
-  </si>
-  <si>
     <t>music</t>
   </si>
   <si>
-    <t>1UWjruNuWA582TCaxQsBbw?si=caBQeK-iSpufSrZRHppWcw</t>
-  </si>
-  <si>
     <t>https://open.spotify.com/album/1UWjruNuWA582TCaxQsBbw?si=caBQeK-iSpufSrZRHppWcw</t>
   </si>
   <si>
     <t>https://open.spotify.com/album/3DB9WITlUNbkGWWHvj94fL?si=3a1bf255ef8a4a8c</t>
   </si>
   <si>
-    <t>3DB9WITlUNbkGWWHvj94fL?si=3a1bf255ef8a4a8c</t>
-  </si>
-  <si>
     <t>https://open.spotify.com/album/2EUxVIRUV8uvItM0b3bpaA?si=nq1UXhYfSGW4AZcj4ADEBA</t>
   </si>
   <si>
-    <t>2EUxVIRUV8uvItM0b3bpaA?si=nq1UXhYfSGW4AZcj4ADEBA</t>
-  </si>
-  <si>
     <t>https://open.spotify.com/album/4gfxAB17Yk3ncXqxvxd77C?si=_EbofBJ1SbWSkrQBpb7eiA</t>
   </si>
   <si>
-    <t>4gfxAB17Yk3ncXqxvxd77C?si=_EbofBJ1SbWSkrQBpb7eiA</t>
-  </si>
-  <si>
     <t>https://open.spotify.com/album/6s2FbDsgTM3PogNwTZfdHL?si=AI9oAfFWSoGIa3jCHw3Azw</t>
   </si>
   <si>
-    <t>6s2FbDsgTM3PogNwTZfdHL?si=AI9oAfFWSoGIa3jCHw3Azw</t>
-  </si>
-  <si>
-    <t>Was ist Was</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/album/1DQZ68JHL3ly3stJ31l1i5?si=93rkjseLRZON-QYdF86EGQ</t>
-  </si>
-  <si>
-    <t>1DQZ68JHL3ly3stJ31l1i5?si=93rkjseLRZON-QYdF86EGQ</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/album/6fger9AdE9C0H8zt3Gcq3N?si=vh0oaehcQ86UBMLrSMcU3g</t>
-  </si>
-  <si>
-    <t>6fger9AdE9C0H8zt3Gcq3N?si=vh0oaehcQ86UBMLrSMcU3g</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/album/57VZXfbpx5VQoD0oOEaKMb?si=l5VX0N9xT0aKWGchqiBjDA</t>
-  </si>
-  <si>
-    <t>57VZXfbpx5VQoD0oOEaKMb?si=l5VX0N9xT0aKWGchqiBjDA</t>
-  </si>
-  <si>
     <t>Olchis</t>
   </si>
   <si>
@@ -198,9 +144,6 @@
     <t>Toggo Radio</t>
   </si>
   <si>
-    <t>3agfnkHCJpThKqifXWXdnc?si=bN0Z4RlJTiqW_erlTsif0w</t>
-  </si>
-  <si>
     <t>https://open.spotify.com/album/3agfnkHCJpThKqifXWXdnc?si=bN0Z4RlJTiqW_erlTsif0w</t>
   </si>
   <si>
@@ -213,45 +156,30 @@
     <t>https://open.spotify.com/album/6k7IrXAqaYTfEJ4YzJvXtz?si=q0Kh38DSRVeWfsj7lCDsgQ</t>
   </si>
   <si>
-    <t>6k7IrXAqaYTfEJ4YzJvXtz?si=q0Kh38DSRVeWfsj7lCDsgQ</t>
-  </si>
-  <si>
     <t>Was ist Was Junior - Pferde Ponys</t>
   </si>
   <si>
     <t>https://open.spotify.com/album/6hvzz7wCE6fGFokyUEhSve?si=EpYubXaFQ4ursslaDijFyQ</t>
   </si>
   <si>
-    <t>6hvzz7wCE6fGFokyUEhSve?si=EpYubXaFQ4ursslaDijFyQ</t>
-  </si>
-  <si>
     <t>Was ist Was Junior - Piraten</t>
   </si>
   <si>
     <t>https://open.spotify.com/album/49Ej9JcVXTjtzszeig3Epm?si=Fg0ijRbsQICr9l-o_m-l2g</t>
   </si>
   <si>
-    <t>49Ej9JcVXTjtzszeig3Epm?si=Fg0ijRbsQICr9l-o_m-l2g</t>
-  </si>
-  <si>
     <t>Was ist Was Junior - Dinosaurier</t>
   </si>
   <si>
     <t>https://open.spotify.com/album/2DMuYgkx2SEDgyNiMc61Ht?si=T7iue8yGSb6QoBY9KSwmMw</t>
   </si>
   <si>
-    <t>2DMuYgkx2SEDgyNiMc61Ht?si=T7iue8yGSb6QoBY9KSwmMw</t>
-  </si>
-  <si>
     <t>Was ist Was Junior - Wale Delfine</t>
   </si>
   <si>
     <t>https://open.spotify.com/album/6FCNX9cYvGqGuLVbvg9VcD?si=OH2mYf3iSv6idHKHyTm4Vw</t>
   </si>
   <si>
-    <t>6FCNX9cYvGqGuLVbvg9VcD?si=OH2mYf3iSv6idHKHyTm4Vw</t>
-  </si>
-  <si>
     <t>Eddie &amp; Dän</t>
   </si>
   <si>
@@ -261,18 +189,12 @@
     <t>https://open.spotify.com/album/6Phy1JysUYXkDFprinZTFU?si=DLW5NJbbR-uP2uyXlOnqVQ</t>
   </si>
   <si>
-    <t>6Phy1JysUYXkDFprinZTFU?si=DLW5NJbbR-uP2uyXlOnqVQ</t>
-  </si>
-  <si>
     <t>Was ist Was Junior - Flughafen</t>
   </si>
   <si>
     <t>https://open.spotify.com/album/6RZMInn9NcEqq8LUk1FSr3?si=HB6FSvKtSIKdZX7GqLykHQ</t>
   </si>
   <si>
-    <t>6RZMInn9NcEqq8LUk1FSr3?si=HB6FSvKtSIKdZX7GqLykHQ</t>
-  </si>
-  <si>
     <t>Was ist Was Junior - Im Zoo</t>
   </si>
   <si>
@@ -282,15 +204,9 @@
     <t>https://open.spotify.com/album/0BVR9okzupLVimOlHvM9cU?si=8SnIWlDZQQ-WO6-zXjwRzA</t>
   </si>
   <si>
-    <t>0BVR9okzupLVimOlHvM9cU?si=8SnIWlDZQQ-WO6-zXjwRzA</t>
-  </si>
-  <si>
     <t>https://open.spotify.com/album/6zvHScikSfubMSkzDijl6E?si=uSYHorouTLKBunJhRdiuug</t>
   </si>
   <si>
-    <t>6zvHScikSfubMSkzDijl6E?si=uSYHorouTLKBunJhRdiuug</t>
-  </si>
-  <si>
     <t>Was ist was Junior - Eisenbahn</t>
   </si>
   <si>
@@ -300,15 +216,6 @@
     <t>artist:Mama Muh album:Mama Muh</t>
   </si>
   <si>
-    <t>Mama Muh geht schwimmen</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/intl-de/album/6LJz7VdDRBJYCxdutpEt8r?si=Dw5zO1JnS12lbSnN_Z2taw</t>
-  </si>
-  <si>
-    <t>6LJz7VdDRBJYCxdutpEt8r?si=Dw5zO1JnS12lbSnN_Z2taw</t>
-  </si>
-  <si>
     <t>artist:Die Olchis album:Die Olchis</t>
   </si>
   <si>
@@ -394,6 +301,69 @@
   </si>
   <si>
     <t>Interner Kommentar, welcher nicht in die data.json integriert wird</t>
+  </si>
+  <si>
+    <t>artistid</t>
+  </si>
+  <si>
+    <t>1JPhbKU3boL67fftU3U1ED</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/intl-de/artist/1JPhbKU3boL67fftU3U1ED</t>
+  </si>
+  <si>
+    <t>3P8jdv34YuU5N2mZAxtAca</t>
+  </si>
+  <si>
+    <t>Rock Weihnachten</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/playlist/3P8jdv34YuU5N2mZAxtAca</t>
+  </si>
+  <si>
+    <t>rss</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Anna und die wilden Tiere</t>
+  </si>
+  <si>
+    <t>nur bei type spotify + rss nutzbar:</t>
+  </si>
+  <si>
+    <t>nur bei category music + other nutzbar</t>
+  </si>
+  <si>
+    <t>Wert nur setzen, wenn aPartofAll = true ist</t>
+  </si>
+  <si>
+    <t>spotify_url</t>
+  </si>
+  <si>
+    <t>Album Cover</t>
+  </si>
+  <si>
+    <t>Label Cover</t>
+  </si>
+  <si>
+    <t>https://feeds.br.de/anna-und-die-wilden-tiere/feed.xml</t>
+  </si>
+  <si>
+    <t>7EPQEUgL5LbEDIRqc5YARW</t>
+  </si>
+  <si>
+    <t>https://assets.laut.fm/ecdf221b2a67d48b8f0dd2ed4a23e0ce?t=_120x120</t>
+  </si>
+  <si>
+    <t>http://stream.laut.fm/minidisco</t>
+  </si>
+  <si>
+    <t>Minidisco</t>
+  </si>
+  <si>
+    <t>Name für Album / Sammlung (type = Spotify, Radio, RSS):</t>
   </si>
   <si>
     <r>
@@ -405,7 +375,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Radio</t>
+      <t xml:space="preserve"> Spotify Query Syntax (type = spotify</t>
     </r>
     <r>
       <rPr>
@@ -415,244 +385,84 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: Attribut für "Menü Radio" -&gt; "Title". Ist der Titel für den Stream</t>
+      <t>)</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Radio:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Attribut für "Menü Radio" -&gt; "Cover Artwork URL"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Audibook und Music:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Attribut für "Menü Audibook und Music" -&gt; "opt. Artist Cover"</t>
-    </r>
-  </si>
-  <si>
-    <t>Audibook und Music:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Audibook und Music: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Wert nur setzen, wenn aPartofAll = true ist</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Audibook und Music: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> In diesem Attribut muss die ID eingetragen werden, wenn es sich um eine Playlist handelt</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Audibook und Music</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Spotify Query Syntax</t>
-    </r>
-  </si>
-  <si>
-    <t>artistid</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Audibook und Music:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Artistid aus Spotify eines Künstlers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Audibook und Music:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Name für Album / Sammlung</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Audibook und Music + Radio</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-AlbumID oder Stream Link</t>
-    </r>
-  </si>
-  <si>
-    <t>showid</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Audibook:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ID für Podcasts</t>
-    </r>
-  </si>
-  <si>
-    <t>6YkiGMyRqAkoKISsTu96bo</t>
-  </si>
-  <si>
-    <t>Finanzfluss</t>
-  </si>
-  <si>
-    <t>Podcast Finanzfluss</t>
-  </si>
-  <si>
-    <t>1JPhbKU3boL67fftU3U1ED</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/intl-de/artist/1JPhbKU3boL67fftU3U1ED</t>
-  </si>
-  <si>
-    <t>3P8jdv34YuU5N2mZAxtAca</t>
-  </si>
-  <si>
-    <t>Rock Weihnachten</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/playlist/3P8jdv34YuU5N2mZAxtAca</t>
+    <t xml:space="preserve">
+Spotify URL (type = spotify)</t>
+  </si>
+  <si>
+    <t>Artist ID aus Spotify URL, Artist ID NUR füllen wenn alles vom Artist geladen werden soll (type = spotify)</t>
+  </si>
+  <si>
+    <t>ID für type = Radio + RSS + spotify (Album ID aus Spotify URL, ID ausfüllen, wenn es sich um ein einzelnes Album handelt)</t>
+  </si>
+  <si>
+    <t>Playlist ID aus Spotify URL, type = spotify</t>
+  </si>
+  <si>
+    <t>Titel für Radio/Stream (type Radio/Stream)</t>
+  </si>
+  <si>
+    <t>5UkoCFXGVib8TIc8cvKtfq</t>
+  </si>
+  <si>
+    <t>3626UDwiaF1YhpqqSn1Deh</t>
+  </si>
+  <si>
+    <t>6bZnwwe52KE9uDlVNQhnyz</t>
+  </si>
+  <si>
+    <t>6ldqnwRlLHxc5qAUCfLm2P</t>
+  </si>
+  <si>
+    <t>029DikZUQus7AGcU2n71tb</t>
+  </si>
+  <si>
+    <t>1UWjruNuWA582TCaxQsBbw</t>
+  </si>
+  <si>
+    <t>3DB9WITlUNbkGWWHvj94fL</t>
+  </si>
+  <si>
+    <t>2EUxVIRUV8uvItM0b3bpaA</t>
+  </si>
+  <si>
+    <t>4gfxAB17Yk3ncXqxvxd77C</t>
+  </si>
+  <si>
+    <t>6s2FbDsgTM3PogNwTZfdHL</t>
+  </si>
+  <si>
+    <t>3agfnkHCJpThKqifXWXdnc</t>
+  </si>
+  <si>
+    <t>6k7IrXAqaYTfEJ4YzJvXtz</t>
+  </si>
+  <si>
+    <t>6hvzz7wCE6fGFokyUEhSve</t>
+  </si>
+  <si>
+    <t>49Ej9JcVXTjtzszeig3Epm</t>
+  </si>
+  <si>
+    <t>2DMuYgkx2SEDgyNiMc61Ht</t>
+  </si>
+  <si>
+    <t>6FCNX9cYvGqGuLVbvg9VcD</t>
+  </si>
+  <si>
+    <t>6Phy1JysUYXkDFprinZTFU</t>
+  </si>
+  <si>
+    <t>6RZMInn9NcEqq8LUk1FSr3</t>
+  </si>
+  <si>
+    <t>0BVR9okzupLVimOlHvM9cU</t>
+  </si>
+  <si>
+    <t>6zvHScikSfubMSkzDijl6E</t>
   </si>
 </sst>
 </file>
@@ -689,7 +499,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -717,6 +527,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -768,9 +590,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill" vertical="center"/>
     </xf>
@@ -783,33 +602,36 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -1121,86 +943,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R100"/>
+  <dimension ref="A1:R96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="K22" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.06640625" customWidth="1"/>
     <col min="2" max="2" width="9.46484375" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" customWidth="1"/>
+    <col min="5" max="5" width="11.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.19921875" customWidth="1"/>
-    <col min="10" max="10" width="27.9296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="29" customWidth="1"/>
-    <col min="13" max="13" width="25.3984375" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" customWidth="1"/>
-    <col min="16" max="16" width="34.796875" style="10" customWidth="1"/>
+    <col min="8" max="10" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" customWidth="1"/>
+    <col min="12" max="13" width="27.19921875" customWidth="1"/>
+    <col min="14" max="14" width="25.3984375" customWidth="1"/>
+    <col min="15" max="15" width="27.19921875" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" customWidth="1"/>
     <col min="17" max="17" width="38.53125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="76.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="17" customFormat="1" ht="71.25">
-      <c r="A1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>118</v>
+    <row r="1" spans="1:18" s="15" customFormat="1" ht="71.25">
+      <c r="A1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1209,43 +1033,43 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>10</v>
@@ -1262,13 +1086,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1278,13 +1102,13 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="7"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="3" t="s">
         <v>0</v>
@@ -1301,10 +1125,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1314,16 +1138,16 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="7"/>
+      <c r="L4" s="20"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="7"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1337,10 +1161,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1350,16 +1174,16 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="7"/>
+      <c r="L5" s="20"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="7"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1373,10 +1197,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1386,16 +1210,16 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="7"/>
+      <c r="L6" s="20"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="7"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -1409,10 +1233,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1422,56 +1246,56 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="7"/>
+      <c r="L7" s="20"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="7"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" s="20" customFormat="1">
-      <c r="A8" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="F8" s="18">
+      <c r="D8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="2">
         <v>30</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18" t="s">
-        <v>136</v>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -1485,10 +1309,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -1497,18 +1321,18 @@
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L9" s="7"/>
+        <v>68</v>
+      </c>
+      <c r="L9" s="20"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="7"/>
+      <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="7"/>
+      <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
@@ -1523,29 +1347,29 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="7"/>
+      <c r="L10" s="20"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O10" s="2"/>
-      <c r="P10" s="7"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1556,13 +1380,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1572,16 +1396,16 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="7"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1592,13 +1416,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1608,16 +1432,16 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="7"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1628,13 +1452,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1644,16 +1468,16 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="7"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1664,13 +1488,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1680,16 +1504,16 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="7"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1700,13 +1524,13 @@
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1716,20 +1540,22 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="7"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1737,97 +1563,113 @@
         <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="K16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" s="20"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="7"/>
+      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="L17" s="20"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="O17" s="2"/>
-      <c r="P17" s="7"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="Q17" s="2"/>
-      <c r="R17" s="3" t="s">
-        <v>46</v>
+      <c r="R17" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="L18" s="20"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="O18" s="2"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="3" t="s">
-        <v>48</v>
+      <c r="N18" s="3"/>
+      <c r="O18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -1835,34 +1677,44 @@
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L19" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="20"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="2" t="s">
@@ -1872,34 +1724,38 @@
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P20" s="11" t="s">
-        <v>104</v>
+      <c r="L20" s="20"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="5" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -1910,36 +1766,38 @@
         <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>105</v>
+      </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P21" s="9" t="s">
+      <c r="L21" s="20"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="Q21" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="P21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q21" s="2"/>
       <c r="R21" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -1947,39 +1805,37 @@
         <v>13</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>108</v>
-      </c>
+      <c r="L22" s="20"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="P22" s="2"/>
       <c r="Q22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>107</v>
+        <v>36</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1987,37 +1843,37 @@
         <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="P23" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="5" t="s">
-        <v>110</v>
+      <c r="L23" s="20"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -2031,31 +1887,31 @@
         <v>9</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+      <c r="L24" s="20"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="O24" s="2"/>
-      <c r="P24" s="7"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="P24" s="2"/>
       <c r="Q24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -2069,31 +1925,31 @@
         <v>9</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
+      <c r="L25" s="20"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="O25" s="2"/>
-      <c r="P25" s="7"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="P25" s="2"/>
       <c r="Q25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -2107,31 +1963,31 @@
         <v>9</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
+      <c r="L26" s="20"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="O26" s="2"/>
-      <c r="P26" s="7"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="P26" s="2"/>
       <c r="Q26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -2142,34 +1998,34 @@
         <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="O27" s="2"/>
-      <c r="P27" s="7"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="P27" s="2"/>
       <c r="Q27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -2183,31 +2039,31 @@
         <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
+      <c r="L28" s="20"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O28" s="2"/>
-      <c r="P28" s="7"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="P28" s="2"/>
       <c r="Q28" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="R28" s="6" t="s">
-        <v>66</v>
+        <v>50</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -2218,34 +2074,34 @@
         <v>7</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="L29" s="20"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="O29" s="2"/>
-      <c r="P29" s="7"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="P29" s="2"/>
       <c r="Q29" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -2259,31 +2115,31 @@
         <v>9</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+      <c r="L30" s="20"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="O30" s="2"/>
-      <c r="P30" s="7"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="P30" s="2"/>
       <c r="Q30" s="2" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -2297,31 +2153,31 @@
         <v>9</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+      <c r="L31" s="20"/>
       <c r="M31" s="2"/>
-      <c r="N31" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="O31" s="2"/>
-      <c r="P31" s="7"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="P31" s="2"/>
       <c r="Q31" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2335,32 +2191,30 @@
         <v>9</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="O32" s="2"/>
-      <c r="P32" s="7"/>
+      <c r="K32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L32" s="20"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="2"/>
       <c r="Q32" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="R32" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="R32" s="3"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="2" t="s">
@@ -2373,32 +2227,30 @@
         <v>9</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="K33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L33" s="20"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" s="7"/>
+      <c r="P33" s="2"/>
       <c r="Q33" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="R33" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="2" t="s">
@@ -2411,30 +2263,28 @@
         <v>9</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L34" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="L34" s="20"/>
       <c r="M34" s="2"/>
-      <c r="N34" s="7"/>
+      <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="R34" s="3"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="2" t="s">
@@ -2447,32 +2297,28 @@
         <v>9</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
+      <c r="K35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L35" s="20"/>
       <c r="M35" s="2"/>
-      <c r="N35" s="7" t="s">
-        <v>89</v>
-      </c>
+      <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="R35" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="2" t="s">
@@ -2485,28 +2331,28 @@
         <v>9</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L36" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="L36" s="20"/>
       <c r="M36" s="2"/>
-      <c r="N36" s="7"/>
+      <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="7"/>
+      <c r="P36" s="2"/>
       <c r="Q36" s="2" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="R36" s="2"/>
     </row>
@@ -2518,179 +2364,129 @@
         <v>7</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="2" t="s">
+      <c r="K37" s="2"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R37" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="20"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="7"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="20"/>
       <c r="M39" s="2"/>
-      <c r="N39" s="7"/>
+      <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F40" s="2">
-        <v>1</v>
-      </c>
-      <c r="G40" s="2">
-        <v>10</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
+      <c r="L40" s="20"/>
       <c r="M40" s="2"/>
-      <c r="N40" s="7"/>
+      <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="N41" s="7"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
       <c r="O41" s="2"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="R41" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="2"/>
@@ -2704,11 +2500,11 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
+      <c r="L42" s="20"/>
       <c r="M42" s="2"/>
-      <c r="N42" s="7"/>
+      <c r="N42" s="2"/>
       <c r="O42" s="2"/>
-      <c r="P42" s="7"/>
+      <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
     </row>
@@ -2724,11 +2520,11 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
+      <c r="L43" s="20"/>
       <c r="M43" s="2"/>
-      <c r="N43" s="7"/>
+      <c r="N43" s="2"/>
       <c r="O43" s="2"/>
-      <c r="P43" s="7"/>
+      <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
     </row>
@@ -2744,11 +2540,11 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
+      <c r="L44" s="20"/>
       <c r="M44" s="2"/>
-      <c r="N44" s="7"/>
+      <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-      <c r="P44" s="7"/>
+      <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
     </row>
@@ -2764,11 +2560,11 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
+      <c r="L45" s="20"/>
       <c r="M45" s="2"/>
-      <c r="N45" s="7"/>
+      <c r="N45" s="2"/>
       <c r="O45" s="2"/>
-      <c r="P45" s="7"/>
+      <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
     </row>
@@ -2784,11 +2580,11 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
+      <c r="L46" s="20"/>
       <c r="M46" s="2"/>
-      <c r="N46" s="7"/>
+      <c r="N46" s="2"/>
       <c r="O46" s="2"/>
-      <c r="P46" s="7"/>
+      <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
@@ -2804,11 +2600,11 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
+      <c r="L47" s="20"/>
       <c r="M47" s="2"/>
-      <c r="N47" s="7"/>
+      <c r="N47" s="2"/>
       <c r="O47" s="2"/>
-      <c r="P47" s="7"/>
+      <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
     </row>
@@ -2824,11 +2620,11 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
+      <c r="L48" s="20"/>
       <c r="M48" s="2"/>
-      <c r="N48" s="7"/>
+      <c r="N48" s="2"/>
       <c r="O48" s="2"/>
-      <c r="P48" s="7"/>
+      <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
     </row>
@@ -2844,11 +2640,11 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
+      <c r="L49" s="20"/>
       <c r="M49" s="2"/>
-      <c r="N49" s="7"/>
+      <c r="N49" s="2"/>
       <c r="O49" s="2"/>
-      <c r="P49" s="7"/>
+      <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
     </row>
@@ -2864,11 +2660,11 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
+      <c r="L50" s="20"/>
       <c r="M50" s="2"/>
-      <c r="N50" s="7"/>
+      <c r="N50" s="2"/>
       <c r="O50" s="2"/>
-      <c r="P50" s="7"/>
+      <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
     </row>
@@ -2884,11 +2680,11 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
+      <c r="L51" s="20"/>
       <c r="M51" s="2"/>
-      <c r="N51" s="7"/>
+      <c r="N51" s="2"/>
       <c r="O51" s="2"/>
-      <c r="P51" s="7"/>
+      <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
     </row>
@@ -2904,11 +2700,11 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
+      <c r="L52" s="20"/>
       <c r="M52" s="2"/>
-      <c r="N52" s="7"/>
+      <c r="N52" s="2"/>
       <c r="O52" s="2"/>
-      <c r="P52" s="7"/>
+      <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
     </row>
@@ -2924,11 +2720,11 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
+      <c r="L53" s="20"/>
       <c r="M53" s="2"/>
-      <c r="N53" s="7"/>
+      <c r="N53" s="2"/>
       <c r="O53" s="2"/>
-      <c r="P53" s="7"/>
+      <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
@@ -2944,11 +2740,11 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
+      <c r="L54" s="20"/>
       <c r="M54" s="2"/>
-      <c r="N54" s="7"/>
+      <c r="N54" s="2"/>
       <c r="O54" s="2"/>
-      <c r="P54" s="7"/>
+      <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
@@ -2964,11 +2760,11 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
+      <c r="L55" s="20"/>
       <c r="M55" s="2"/>
-      <c r="N55" s="7"/>
+      <c r="N55" s="2"/>
       <c r="O55" s="2"/>
-      <c r="P55" s="7"/>
+      <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
@@ -2984,11 +2780,11 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
+      <c r="L56" s="20"/>
       <c r="M56" s="2"/>
-      <c r="N56" s="7"/>
+      <c r="N56" s="2"/>
       <c r="O56" s="2"/>
-      <c r="P56" s="7"/>
+      <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
     </row>
@@ -3004,11 +2800,11 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
+      <c r="L57" s="20"/>
       <c r="M57" s="2"/>
-      <c r="N57" s="7"/>
+      <c r="N57" s="2"/>
       <c r="O57" s="2"/>
-      <c r="P57" s="7"/>
+      <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
@@ -3024,11 +2820,11 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
+      <c r="L58" s="20"/>
       <c r="M58" s="2"/>
-      <c r="N58" s="7"/>
+      <c r="N58" s="2"/>
       <c r="O58" s="2"/>
-      <c r="P58" s="7"/>
+      <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
     </row>
@@ -3044,11 +2840,11 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
+      <c r="L59" s="20"/>
       <c r="M59" s="2"/>
-      <c r="N59" s="7"/>
+      <c r="N59" s="2"/>
       <c r="O59" s="2"/>
-      <c r="P59" s="7"/>
+      <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
     </row>
@@ -3064,11 +2860,11 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
+      <c r="L60" s="20"/>
       <c r="M60" s="2"/>
-      <c r="N60" s="7"/>
+      <c r="N60" s="2"/>
       <c r="O60" s="2"/>
-      <c r="P60" s="7"/>
+      <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
@@ -3084,11 +2880,11 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
+      <c r="L61" s="20"/>
       <c r="M61" s="2"/>
-      <c r="N61" s="7"/>
+      <c r="N61" s="2"/>
       <c r="O61" s="2"/>
-      <c r="P61" s="7"/>
+      <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
@@ -3104,11 +2900,11 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
+      <c r="L62" s="20"/>
       <c r="M62" s="2"/>
-      <c r="N62" s="7"/>
+      <c r="N62" s="2"/>
       <c r="O62" s="2"/>
-      <c r="P62" s="7"/>
+      <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
     </row>
@@ -3124,11 +2920,11 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
+      <c r="L63" s="20"/>
       <c r="M63" s="2"/>
-      <c r="N63" s="7"/>
+      <c r="N63" s="2"/>
       <c r="O63" s="2"/>
-      <c r="P63" s="7"/>
+      <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
     </row>
@@ -3144,11 +2940,11 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
+      <c r="L64" s="20"/>
       <c r="M64" s="2"/>
-      <c r="N64" s="7"/>
+      <c r="N64" s="2"/>
       <c r="O64" s="2"/>
-      <c r="P64" s="7"/>
+      <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
     </row>
@@ -3164,11 +2960,11 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
+      <c r="L65" s="20"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="7"/>
+      <c r="N65" s="2"/>
       <c r="O65" s="2"/>
-      <c r="P65" s="7"/>
+      <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
     </row>
@@ -3184,11 +2980,11 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
+      <c r="L66" s="20"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="7"/>
+      <c r="N66" s="2"/>
       <c r="O66" s="2"/>
-      <c r="P66" s="7"/>
+      <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
     </row>
@@ -3204,11 +3000,11 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
+      <c r="L67" s="20"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="7"/>
+      <c r="N67" s="2"/>
       <c r="O67" s="2"/>
-      <c r="P67" s="7"/>
+      <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
     </row>
@@ -3224,11 +3020,11 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
+      <c r="L68" s="20"/>
       <c r="M68" s="2"/>
-      <c r="N68" s="7"/>
+      <c r="N68" s="2"/>
       <c r="O68" s="2"/>
-      <c r="P68" s="7"/>
+      <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
     </row>
@@ -3244,11 +3040,11 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
-      <c r="L69" s="2"/>
+      <c r="L69" s="20"/>
       <c r="M69" s="2"/>
-      <c r="N69" s="7"/>
+      <c r="N69" s="2"/>
       <c r="O69" s="2"/>
-      <c r="P69" s="7"/>
+      <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
@@ -3264,11 +3060,11 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
+      <c r="L70" s="20"/>
       <c r="M70" s="2"/>
-      <c r="N70" s="7"/>
+      <c r="N70" s="2"/>
       <c r="O70" s="2"/>
-      <c r="P70" s="7"/>
+      <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
     </row>
@@ -3284,11 +3080,11 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
+      <c r="L71" s="20"/>
       <c r="M71" s="2"/>
-      <c r="N71" s="7"/>
+      <c r="N71" s="2"/>
       <c r="O71" s="2"/>
-      <c r="P71" s="7"/>
+      <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
     </row>
@@ -3304,11 +3100,11 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
-      <c r="L72" s="2"/>
+      <c r="L72" s="20"/>
       <c r="M72" s="2"/>
-      <c r="N72" s="7"/>
+      <c r="N72" s="2"/>
       <c r="O72" s="2"/>
-      <c r="P72" s="7"/>
+      <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
     </row>
@@ -3324,11 +3120,11 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
+      <c r="L73" s="20"/>
       <c r="M73" s="2"/>
-      <c r="N73" s="7"/>
+      <c r="N73" s="2"/>
       <c r="O73" s="2"/>
-      <c r="P73" s="7"/>
+      <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
     </row>
@@ -3344,11 +3140,11 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
-      <c r="L74" s="2"/>
+      <c r="L74" s="20"/>
       <c r="M74" s="2"/>
-      <c r="N74" s="7"/>
+      <c r="N74" s="2"/>
       <c r="O74" s="2"/>
-      <c r="P74" s="7"/>
+      <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
       <c r="R74" s="2"/>
     </row>
@@ -3364,11 +3160,11 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
-      <c r="L75" s="2"/>
+      <c r="L75" s="20"/>
       <c r="M75" s="2"/>
-      <c r="N75" s="7"/>
+      <c r="N75" s="2"/>
       <c r="O75" s="2"/>
-      <c r="P75" s="7"/>
+      <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
       <c r="R75" s="2"/>
     </row>
@@ -3384,11 +3180,11 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
+      <c r="L76" s="20"/>
       <c r="M76" s="2"/>
-      <c r="N76" s="7"/>
+      <c r="N76" s="2"/>
       <c r="O76" s="2"/>
-      <c r="P76" s="7"/>
+      <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
       <c r="R76" s="2"/>
     </row>
@@ -3404,11 +3200,11 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
-      <c r="L77" s="2"/>
+      <c r="L77" s="20"/>
       <c r="M77" s="2"/>
-      <c r="N77" s="7"/>
+      <c r="N77" s="2"/>
       <c r="O77" s="2"/>
-      <c r="P77" s="7"/>
+      <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
@@ -3424,11 +3220,11 @@
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
+      <c r="L78" s="20"/>
       <c r="M78" s="2"/>
-      <c r="N78" s="7"/>
+      <c r="N78" s="2"/>
       <c r="O78" s="2"/>
-      <c r="P78" s="7"/>
+      <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
     </row>
@@ -3444,11 +3240,11 @@
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
+      <c r="L79" s="20"/>
       <c r="M79" s="2"/>
-      <c r="N79" s="7"/>
+      <c r="N79" s="2"/>
       <c r="O79" s="2"/>
-      <c r="P79" s="7"/>
+      <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
       <c r="R79" s="2"/>
     </row>
@@ -3464,11 +3260,11 @@
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
+      <c r="L80" s="20"/>
       <c r="M80" s="2"/>
-      <c r="N80" s="7"/>
+      <c r="N80" s="2"/>
       <c r="O80" s="2"/>
-      <c r="P80" s="7"/>
+      <c r="P80" s="2"/>
       <c r="Q80" s="2"/>
       <c r="R80" s="2"/>
     </row>
@@ -3484,11 +3280,11 @@
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
-      <c r="L81" s="2"/>
+      <c r="L81" s="20"/>
       <c r="M81" s="2"/>
-      <c r="N81" s="7"/>
+      <c r="N81" s="2"/>
       <c r="O81" s="2"/>
-      <c r="P81" s="7"/>
+      <c r="P81" s="2"/>
       <c r="Q81" s="2"/>
       <c r="R81" s="2"/>
     </row>
@@ -3504,11 +3300,11 @@
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
+      <c r="L82" s="20"/>
       <c r="M82" s="2"/>
-      <c r="N82" s="7"/>
+      <c r="N82" s="2"/>
       <c r="O82" s="2"/>
-      <c r="P82" s="7"/>
+      <c r="P82" s="2"/>
       <c r="Q82" s="2"/>
       <c r="R82" s="2"/>
     </row>
@@ -3524,11 +3320,11 @@
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
-      <c r="L83" s="2"/>
+      <c r="L83" s="20"/>
       <c r="M83" s="2"/>
-      <c r="N83" s="7"/>
+      <c r="N83" s="2"/>
       <c r="O83" s="2"/>
-      <c r="P83" s="7"/>
+      <c r="P83" s="2"/>
       <c r="Q83" s="2"/>
       <c r="R83" s="2"/>
     </row>
@@ -3544,11 +3340,11 @@
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
-      <c r="L84" s="2"/>
+      <c r="L84" s="20"/>
       <c r="M84" s="2"/>
-      <c r="N84" s="7"/>
+      <c r="N84" s="2"/>
       <c r="O84" s="2"/>
-      <c r="P84" s="7"/>
+      <c r="P84" s="2"/>
       <c r="Q84" s="2"/>
       <c r="R84" s="2"/>
     </row>
@@ -3564,11 +3360,11 @@
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
-      <c r="L85" s="2"/>
+      <c r="L85" s="20"/>
       <c r="M85" s="2"/>
-      <c r="N85" s="7"/>
+      <c r="N85" s="2"/>
       <c r="O85" s="2"/>
-      <c r="P85" s="7"/>
+      <c r="P85" s="2"/>
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
@@ -3584,11 +3380,11 @@
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
+      <c r="L86" s="20"/>
       <c r="M86" s="2"/>
-      <c r="N86" s="7"/>
+      <c r="N86" s="2"/>
       <c r="O86" s="2"/>
-      <c r="P86" s="7"/>
+      <c r="P86" s="2"/>
       <c r="Q86" s="2"/>
       <c r="R86" s="2"/>
     </row>
@@ -3604,11 +3400,11 @@
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
-      <c r="L87" s="2"/>
+      <c r="L87" s="20"/>
       <c r="M87" s="2"/>
-      <c r="N87" s="7"/>
+      <c r="N87" s="2"/>
       <c r="O87" s="2"/>
-      <c r="P87" s="7"/>
+      <c r="P87" s="2"/>
       <c r="Q87" s="2"/>
       <c r="R87" s="2"/>
     </row>
@@ -3624,11 +3420,11 @@
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
-      <c r="L88" s="2"/>
+      <c r="L88" s="20"/>
       <c r="M88" s="2"/>
-      <c r="N88" s="7"/>
+      <c r="N88" s="2"/>
       <c r="O88" s="2"/>
-      <c r="P88" s="7"/>
+      <c r="P88" s="2"/>
       <c r="Q88" s="2"/>
       <c r="R88" s="2"/>
     </row>
@@ -3644,11 +3440,11 @@
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
+      <c r="L89" s="20"/>
       <c r="M89" s="2"/>
-      <c r="N89" s="7"/>
+      <c r="N89" s="2"/>
       <c r="O89" s="2"/>
-      <c r="P89" s="7"/>
+      <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
       <c r="R89" s="2"/>
     </row>
@@ -3664,11 +3460,11 @@
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
-      <c r="L90" s="2"/>
+      <c r="L90" s="20"/>
       <c r="M90" s="2"/>
-      <c r="N90" s="7"/>
+      <c r="N90" s="2"/>
       <c r="O90" s="2"/>
-      <c r="P90" s="7"/>
+      <c r="P90" s="2"/>
       <c r="Q90" s="2"/>
       <c r="R90" s="2"/>
     </row>
@@ -3684,11 +3480,11 @@
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
-      <c r="L91" s="2"/>
+      <c r="L91" s="20"/>
       <c r="M91" s="2"/>
-      <c r="N91" s="7"/>
+      <c r="N91" s="2"/>
       <c r="O91" s="2"/>
-      <c r="P91" s="7"/>
+      <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
       <c r="R91" s="2"/>
     </row>
@@ -3704,11 +3500,11 @@
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
-      <c r="L92" s="2"/>
+      <c r="L92" s="20"/>
       <c r="M92" s="2"/>
-      <c r="N92" s="7"/>
+      <c r="N92" s="2"/>
       <c r="O92" s="2"/>
-      <c r="P92" s="7"/>
+      <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
       <c r="R92" s="2"/>
     </row>
@@ -3724,11 +3520,11 @@
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
+      <c r="L93" s="20"/>
       <c r="M93" s="2"/>
-      <c r="N93" s="7"/>
+      <c r="N93" s="2"/>
       <c r="O93" s="2"/>
-      <c r="P93" s="7"/>
+      <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
@@ -3744,11 +3540,11 @@
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
-      <c r="L94" s="2"/>
+      <c r="L94" s="20"/>
       <c r="M94" s="2"/>
-      <c r="N94" s="7"/>
+      <c r="N94" s="2"/>
       <c r="O94" s="2"/>
-      <c r="P94" s="7"/>
+      <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
       <c r="R94" s="2"/>
     </row>
@@ -3764,11 +3560,11 @@
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
-      <c r="L95" s="2"/>
+      <c r="L95" s="20"/>
       <c r="M95" s="2"/>
-      <c r="N95" s="7"/>
+      <c r="N95" s="2"/>
       <c r="O95" s="2"/>
-      <c r="P95" s="7"/>
+      <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
       <c r="R95" s="2"/>
     </row>
@@ -3784,136 +3580,51 @@
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
-      <c r="L96" s="2"/>
+      <c r="L96" s="20"/>
       <c r="M96" s="2"/>
-      <c r="N96" s="7"/>
+      <c r="N96" s="2"/>
       <c r="O96" s="2"/>
-      <c r="P96" s="7"/>
+      <c r="P96" s="2"/>
       <c r="Q96" s="2"/>
       <c r="R96" s="2"/>
     </row>
-    <row r="97" spans="1:18">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
-      <c r="L97" s="2"/>
-      <c r="M97" s="2"/>
-      <c r="N97" s="7"/>
-      <c r="O97" s="2"/>
-      <c r="P97" s="7"/>
-      <c r="Q97" s="2"/>
-      <c r="R97" s="2"/>
-    </row>
-    <row r="98" spans="1:18">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-      <c r="K98" s="2"/>
-      <c r="L98" s="2"/>
-      <c r="M98" s="2"/>
-      <c r="N98" s="7"/>
-      <c r="O98" s="2"/>
-      <c r="P98" s="7"/>
-      <c r="Q98" s="2"/>
-      <c r="R98" s="2"/>
-    </row>
-    <row r="99" spans="1:18">
-      <c r="A99" s="2"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-      <c r="J99" s="2"/>
-      <c r="K99" s="2"/>
-      <c r="L99" s="2"/>
-      <c r="M99" s="2"/>
-      <c r="N99" s="7"/>
-      <c r="O99" s="2"/>
-      <c r="P99" s="7"/>
-      <c r="Q99" s="2"/>
-      <c r="R99" s="2"/>
-    </row>
-    <row r="100" spans="1:18">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
-      <c r="K100" s="2"/>
-      <c r="L100" s="2"/>
-      <c r="M100" s="2"/>
-      <c r="N100" s="7"/>
-      <c r="O100" s="2"/>
-      <c r="P100" s="7"/>
-      <c r="Q100" s="2"/>
-      <c r="R100" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:R29" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:R38" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R12">
     <sortCondition ref="C3:C12"/>
   </sortState>
-  <conditionalFormatting sqref="F3:G40">
-    <cfRule type="expression" dxfId="5" priority="2">
+  <conditionalFormatting sqref="F3:G96">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$E3="false"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:I11">
-    <cfRule type="expression" dxfId="4" priority="6">
+  <conditionalFormatting sqref="H11:J11 L11">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>AND($B11="tunein",$C11="radio")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>AND($B11="spotify",$C11="playlist")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:L20 O20 H3:M10 O3:O10">
-    <cfRule type="expression" dxfId="2" priority="19">
+  <conditionalFormatting sqref="H3:L8 N3:N10 P3:P10 M8 O8:O9 H9:M9 H10:L10 H17 K17:M17 P17">
+    <cfRule type="expression" dxfId="1" priority="20">
       <formula>AND($B3="spotify",$C3="playlist")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10">
-    <cfRule type="expression" dxfId="1" priority="3">
+  <conditionalFormatting sqref="P10">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>AND(G10="spotify",#REF!="playlist")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:G100">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$E41="false"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B100" xr:uid="{5EF866BB-3506-4246-ABAF-7F3DDCEDCB12}">
-      <formula1>"spotify,radio"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:E100" xr:uid="{87F41B23-0A1D-4FE1-89B5-AC2C998105E0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:E96" xr:uid="{87F41B23-0A1D-4FE1-89B5-AC2C998105E0}">
       <formula1>"false,true"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C100" xr:uid="{6E878360-F62C-474A-83F6-2BDF54B993DF}">
-      <formula1>"audiobook,music,radio"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C96" xr:uid="{6E878360-F62C-474A-83F6-2BDF54B993DF}">
+      <formula1>"audiobook,music,other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B96" xr:uid="{48748F27-CCD7-43B0-87E4-E49B4BED4FA5}">
+      <formula1>"spotify,radio,rss"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -3928,24 +3639,28 @@
     <hyperlink ref="R13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="R14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="R15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="R16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="R17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="R18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="R25" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="R26" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="R28" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="R29" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="R30" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="R31" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="R32" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="R33" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="R35" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="P21" r:id="rId24" xr:uid="{94A89889-0453-4B10-8348-141CB9A1C640}"/>
-    <hyperlink ref="P20" r:id="rId25" xr:uid="{451774B7-DD21-423C-90D2-EF2EDE5E5441}"/>
-    <hyperlink ref="P23" r:id="rId26" xr:uid="{78A82A69-93F9-42C8-8DA2-2A6817303156}"/>
-    <hyperlink ref="R41" r:id="rId27" xr:uid="{41C795C4-A372-4F58-A046-8B2C5EC939CB}"/>
+    <hyperlink ref="R23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="R24" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="R26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="R27" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="R28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="R29" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="R30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="R31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="R37" r:id="rId20" xr:uid="{41C795C4-A372-4F58-A046-8B2C5EC939CB}"/>
+    <hyperlink ref="J18" r:id="rId21" xr:uid="{92FCA0FD-BE25-49CE-B556-8914774122B4}"/>
+    <hyperlink ref="J20" r:id="rId22" xr:uid="{87F8926B-5E8A-4A7D-99C2-50F55565EF93}"/>
+    <hyperlink ref="J17" r:id="rId23" xr:uid="{E45E18B8-4020-49CB-823E-CC226A1932D5}"/>
+    <hyperlink ref="J21" r:id="rId24" display="https://deref-web.de/mail/client/Xq35I6CVxd8/dereferrer/?redirectUrl=https%3A%2F%2Fassets.laut.fm%2Fecdf221b2a67d48b8f0dd2ed4a23e0ce%3Ft%3D_120x120" xr:uid="{A4A22E49-59D0-4B11-BED4-187CB6C5C6E8}"/>
+    <hyperlink ref="O21" r:id="rId25" display="https://deref-web.de/mail/client/4t0Ghp40Xos/dereferrer/?redirectUrl=http%3A%2F%2Fstream.laut.fm%2Fminidisco" xr:uid="{F0A2F1AA-B836-41D1-908A-F3872A56E77C}"/>
+    <hyperlink ref="O20" r:id="rId26" xr:uid="{82D2488B-5C08-4520-9032-E78AFC97B910}"/>
+    <hyperlink ref="O18" r:id="rId27" xr:uid="{DF49B130-CDB5-4A64-BC5D-8AEFEF6FA9EC}"/>
+    <hyperlink ref="I18" r:id="rId28" xr:uid="{733AA51E-22B0-41FD-B24B-8161A5F4DD72}"/>
+    <hyperlink ref="I20" r:id="rId29" xr:uid="{E594A5C4-13CD-41D8-9A8A-14ED3258F0DF}"/>
+    <hyperlink ref="I17" r:id="rId30" xr:uid="{B71A904A-A27D-44D2-87F8-57A45402AA94}"/>
+    <hyperlink ref="I21" r:id="rId31" display="https://deref-web.de/mail/client/Xq35I6CVxd8/dereferrer/?redirectUrl=https%3A%2F%2Fassets.laut.fm%2Fecdf221b2a67d48b8f0dd2ed4a23e0ce%3Ft%3D_120x120" xr:uid="{44D65D25-6294-4798-9E13-86C157CEBD2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>